<commit_message>
Correcciones reportes/leyes simples y compuestos
</commit_message>
<xml_diff>
--- a/assets/info/plantilla-repcompuestos-leyes.xlsx
+++ b/assets/info/plantilla-repcompuestos-leyes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
   <si>
     <t xml:space="preserve">REPORTES LEYES</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t xml:space="preserve">ESTADO [%]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CODIGO</t>
   </si>
   <si>
     <t xml:space="preserve">DESCRIPCION DE LA LEY</t>
@@ -444,13 +447,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>66600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>29160</xdr:rowOff>
+      <xdr:rowOff>29520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>983880</xdr:colOff>
+      <xdr:colOff>982440</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>47520</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -463,8 +466,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="66600" y="581400"/>
-          <a:ext cx="3587400" cy="1123200"/>
+          <a:off x="66600" y="581760"/>
+          <a:ext cx="3585960" cy="1121760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -486,13 +489,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>66600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:rowOff>29520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>923400</xdr:colOff>
+      <xdr:colOff>921960</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -505,8 +508,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="66600" y="581040"/>
-          <a:ext cx="3526920" cy="1256760"/>
+          <a:off x="66600" y="581760"/>
+          <a:ext cx="3525480" cy="1255320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -528,13 +531,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>66600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:rowOff>29520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>732960</xdr:colOff>
+      <xdr:colOff>731520</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>228240</xdr:rowOff>
+      <xdr:rowOff>227520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -547,8 +550,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="66600" y="581040"/>
-          <a:ext cx="3336480" cy="1304280"/>
+          <a:off x="66600" y="581760"/>
+          <a:ext cx="3335040" cy="1302840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -568,30 +571,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="43.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="46.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="59.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="59.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="44.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="40.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="5" width="29.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="5" width="34.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="5" width="43.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="5" width="40.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="5" width="37.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="17" style="5" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="44.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="44.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="40.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="5" width="25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="5" width="29.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="5" width="34.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="5" width="43.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="5" width="40.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="5" width="37.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="18" style="5" width="11.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -608,24 +612,28 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
     </row>
     <row r="2" s="5" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" s="5" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E3" s="8"/>
       <c r="F3" s="9"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" s="5" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
@@ -652,7 +660,7 @@
       <c r="H5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="12" t="s">
         <v>9</v>
       </c>
       <c r="J5" s="11" t="s">
@@ -670,34 +678,37 @@
       <c r="N5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="11"/>
+      <c r="O5" s="11" t="s">
+        <v>15</v>
+      </c>
       <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
-  <conditionalFormatting sqref="H6:H1048576 H1">
+  <conditionalFormatting sqref="I6:I1048576 I1">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Reforma Electoral" dxfId="0">
-      <formula>NOT(ISERROR(SEARCH("Reforma Electoral",H1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H4 H6:H1048576">
+      <formula>NOT(ISERROR(SEARCH("Reforma Electoral",I1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I4 I6:I1048576">
     <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Censo" dxfId="1">
-      <formula>NOT(ISERROR(SEARCH("Censo",H1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Censo",I1)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Institucionalidad Democratica" dxfId="2">
-      <formula>NOT(ISERROR(SEARCH("Institucionalidad Democratica",H1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5">
+      <formula>NOT(ISERROR(SEARCH("Institucionalidad Democratica",I1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
     <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Censo" dxfId="3">
-      <formula>NOT(ISERROR(SEARCH("Censo",H5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5">
+      <formula>NOT(ISERROR(SEARCH("Censo",I5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
     <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Institucionalidad Democratica" dxfId="4">
-      <formula>NOT(ISERROR(SEARCH("Institucionalidad Democratica",H5)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Institucionalidad Democratica",I5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -716,30 +727,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:AMJ5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="43.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="41.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="41.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="46.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="59.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="59.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="42.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="26.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="23.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="29.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="5" width="34.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="5" width="43.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="5" width="34.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="5" width="43.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="5" width="40.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="5" width="37.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="5" width="11.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="16" style="5" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -761,16 +773,19 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="13"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" s="5" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
       <c r="F3" s="7"/>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" s="5" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
+      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
@@ -792,22 +807,22 @@
         <v>7</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
@@ -856,30 +871,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:AMJ5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="43.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="46.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="59.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="59.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="48.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="32.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="48.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="32.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="36.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="29.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="5" width="38.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="5" width="43.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="5" width="43.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="5" width="40.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="5" width="37.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="5" width="11.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="16" style="5" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -901,16 +917,19 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="13"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" s="5" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
       <c r="F3" s="7"/>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" s="5" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
+      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
@@ -932,25 +951,25 @@
         <v>7</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>

</xml_diff>